<commit_message>
menyempurnakan fitur upload batch
</commit_message>
<xml_diff>
--- a/public/folderResource/Format_Jadwal_SemPro_Sinkronus_Daring.xlsx
+++ b/public/folderResource/Format_Jadwal_SemPro_Sinkronus_Daring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-7\htdocs\thesis-2022\public\folderResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF01EEF-B2DE-4E7D-AB18-74EC6BF3301A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321E1AA-37E7-4E13-884A-2663E5DFE2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,13 @@
     <t>Link Konferensi</t>
   </si>
   <si>
-    <t>Inisial Dosen Penguji 1</t>
-  </si>
-  <si>
-    <t>Inisial Dosen Penguji 2</t>
-  </si>
-  <si>
     <t>NPM</t>
+  </si>
+  <si>
+    <t>Inisial Dosen Reviewer 1</t>
+  </si>
+  <si>
+    <t>Inisial Dosen Reviewer 2</t>
   </si>
 </sst>
 </file>
@@ -361,21 +361,21 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="19.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -384,10 +384,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>